<commit_message>
add more questions in Games Anime
</commit_message>
<xml_diff>
--- a/Questions/advertise.xlsx
+++ b/Questions/advertise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/My Works/Rails/speedQuizRails/Questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1691758F-7938-CA45-9D53-51ADE7CDD534}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5F70A9-2028-7C45-AA83-8B3CBAC08F8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{F3CEA977-5101-6F4B-A7FE-0516B29D62EF}"/>
+    <workbookView xWindow="28800" yWindow="3100" windowWidth="19200" windowHeight="14900" xr2:uid="{F3CEA977-5101-6F4B-A7FE-0516B29D62EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,329 +35,333 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
   <si>
+    <t>빠삐코</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쿠우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이가탄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>새우깡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신라면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오로라민씨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오레오</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동원참치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연두</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이마트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아웃백</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>첵스초코</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>롤리팝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아몰레드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빅맥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>짜파게티</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>너구리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>팔도비빔면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오란씨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>트로피카나</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>초록매실</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미녀는석류를좋아해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>널깨물어주고싶어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>베스킨라빈스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>베스킨라빈스31 베라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>show</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KT 쑈 쇼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>산와머니</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배칠수꽃배달</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>꽃배달</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">앞뒤가똑같은전화번호1577-1577대리운전 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1577, 앞뒤가똑같은전화번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>여명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>여명808</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울사이버대학</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시원스쿨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T6Ua34lPh_0</t>
+  </si>
+  <si>
+    <t>vXqlaz_8FH4</t>
+  </si>
+  <si>
+    <t>6eH86klRbME</t>
+  </si>
+  <si>
+    <t>DnrrZNkj7Ok</t>
+  </si>
+  <si>
+    <t>QMwci5_4VI0</t>
+  </si>
+  <si>
+    <t>진라면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xCXxFAnzXn4</t>
+  </si>
+  <si>
+    <t>ZM-aogMDP3s</t>
+  </si>
+  <si>
+    <t>8hAVAmOJTr8</t>
+  </si>
+  <si>
+    <t>cPJiPphm8tg</t>
+  </si>
+  <si>
+    <t>야놀자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ejW40LEwxGY</t>
+  </si>
+  <si>
+    <t>ds3iedhVZaQ</t>
+  </si>
+  <si>
+    <t>bAvUzRQDv1c</t>
+  </si>
+  <si>
+    <t>SEhQID2zB3o</t>
+  </si>
+  <si>
+    <t>vUqpAIGecUo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ltPyf9IU3dI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IzgRsRIHZfw</t>
+  </si>
+  <si>
+    <t>구아바</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>야나두</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스크류바</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fp24y7pYZUY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l_gcVPx1PPU</t>
+  </si>
+  <si>
+    <t>xHusEaBbMHU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>puWvOjgp5SU</t>
+  </si>
+  <si>
+    <t>zMSzwGxfOFI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FB9N30TAXX0</t>
+  </si>
+  <si>
+    <t>포카리스웨트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bckLRglL5qg</t>
+  </si>
+  <si>
+    <t>QCrYIjuc8rQ</t>
+  </si>
+  <si>
+    <t>D5pwzTUVTGM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JXxMsQ-2uOA</t>
+  </si>
+  <si>
+    <t>MXG2L-Li3cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6Nhaif5EPj4</t>
+  </si>
+  <si>
+    <t>QnUX1Ef-Vyw</t>
+  </si>
+  <si>
+    <t>jPU3DgMl1xU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vqtHnuVzwoI</t>
+  </si>
+  <si>
+    <t>nRXMcg4313E</t>
+  </si>
+  <si>
+    <t>대성마이맥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마이맥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0zKTiGEwLps</t>
+  </si>
+  <si>
+    <t>ogAhXWZaAJQ</t>
+  </si>
+  <si>
+    <t>n6inJAVe_L4</t>
+  </si>
+  <si>
+    <t>델몬트화이트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XxaQ0EMc88U</t>
+  </si>
+  <si>
+    <t>LJcJJ64N4nc</t>
+  </si>
+  <si>
+    <t>Al4C3wuW1_8</t>
+  </si>
+  <si>
+    <t>포카리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>src</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>startTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>answer</t>
-  </si>
-  <si>
-    <t>answer keyword</t>
-  </si>
-  <si>
-    <t>빠삐코</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>쿠우</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이가탄</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>새우깡</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>신라면</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오로라민씨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오레오</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동원참치</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>연두</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이마트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아웃백</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>첵스초코</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>롤리팝</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아이디</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아몰레드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>빅맥</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>짜파게티</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>너구리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>팔도비빔면</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오란씨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>트로피카나</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>초록매실</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>미녀는석류를좋아해</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>널깨물어주고싶어</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>베스킨라빈스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>베스킨라빈스31 베라</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>show</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>KT 쑈 쇼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>산와머니</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>배칠수꽃배달</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>꽃배달</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">앞뒤가똑같은전화번호1577-1577대리운전 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1577, 앞뒤가똑같은전화번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>여명</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>여명808</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>서울사이버대학</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>시원스쿨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>T6Ua34lPh_0</t>
-  </si>
-  <si>
-    <t>vXqlaz_8FH4</t>
-  </si>
-  <si>
-    <t>6eH86klRbME</t>
-  </si>
-  <si>
-    <t>DnrrZNkj7Ok</t>
-  </si>
-  <si>
-    <t>QMwci5_4VI0</t>
-  </si>
-  <si>
-    <t>진라면</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>xCXxFAnzXn4</t>
-  </si>
-  <si>
-    <t>ZM-aogMDP3s</t>
-  </si>
-  <si>
-    <t>8hAVAmOJTr8</t>
-  </si>
-  <si>
-    <t>cPJiPphm8tg</t>
-  </si>
-  <si>
-    <t>야놀자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ejW40LEwxGY</t>
-  </si>
-  <si>
-    <t>ds3iedhVZaQ</t>
-  </si>
-  <si>
-    <t>bAvUzRQDv1c</t>
-  </si>
-  <si>
-    <t>SEhQID2zB3o</t>
-  </si>
-  <si>
-    <t>vUqpAIGecUo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ltPyf9IU3dI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IzgRsRIHZfw</t>
-  </si>
-  <si>
-    <t>구아바</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>야나두</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스크류바</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fp24y7pYZUY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>l_gcVPx1PPU</t>
-  </si>
-  <si>
-    <t>xHusEaBbMHU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>puWvOjgp5SU</t>
-  </si>
-  <si>
-    <t>zMSzwGxfOFI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FB9N30TAXX0</t>
-  </si>
-  <si>
-    <t>포카리스웨트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bckLRglL5qg</t>
-  </si>
-  <si>
-    <t>QCrYIjuc8rQ</t>
-  </si>
-  <si>
-    <t>D5pwzTUVTGM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JXxMsQ-2uOA</t>
-  </si>
-  <si>
-    <t>MXG2L-Li3cs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6Nhaif5EPj4</t>
-  </si>
-  <si>
-    <t>QnUX1Ef-Vyw</t>
-  </si>
-  <si>
-    <t>jPU3DgMl1xU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vqtHnuVzwoI</t>
-  </si>
-  <si>
-    <t>nRXMcg4313E</t>
-  </si>
-  <si>
-    <t>대성마이맥</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>마이맥</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0zKTiGEwLps</t>
-  </si>
-  <si>
-    <t>ogAhXWZaAJQ</t>
-  </si>
-  <si>
-    <t>n6inJAVe_L4</t>
-  </si>
-  <si>
-    <t>델몬트화이트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>XxaQ0EMc88U</t>
-  </si>
-  <si>
-    <t>LJcJJ64N4nc</t>
-  </si>
-  <si>
-    <t>Al4C3wuW1_8</t>
-  </si>
-  <si>
-    <t>포카리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>answerKeyword</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -365,7 +369,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -380,12 +384,6 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -426,18 +424,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -758,7 +753,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -770,19 +765,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -790,13 +785,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -804,13 +799,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -818,13 +813,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -832,13 +827,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -846,13 +841,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -860,13 +855,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -874,13 +869,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -888,13 +883,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -902,13 +897,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -916,13 +911,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -930,13 +925,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C12">
         <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -944,27 +939,27 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C13">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>57</v>
+      <c r="B14" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -972,16 +967,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -989,13 +984,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1003,13 +998,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1017,13 +1012,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C18">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1031,13 +1026,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1045,13 +1040,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C20">
         <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1059,13 +1054,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1073,13 +1068,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1087,16 +1082,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1104,13 +1099,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1118,16 +1113,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1135,16 +1130,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C26">
         <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E26" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1152,13 +1147,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1166,16 +1161,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E28" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1183,16 +1178,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E29" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1200,16 +1195,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E30" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1217,13 +1212,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1231,13 +1226,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1245,13 +1240,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1259,13 +1254,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1273,16 +1268,16 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E35" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1290,13 +1285,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1304,13 +1299,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1318,16 +1313,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C38">
         <v>3</v>
       </c>
       <c r="D38" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E38" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1335,16 +1330,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E39" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>